<commit_message>
MVC UPDATE DAB H3
</commit_message>
<xml_diff>
--- a/temp_doc/PESERTA UJIAN FIX ADMIN XII FIX.xlsx
+++ b/temp_doc/PESERTA UJIAN FIX ADMIN XII FIX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/cbt2.0admin/temp_doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C049B5-EB85-A444-AA76-D19BE8F14A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD880CEA-93C7-FA4F-9909-C4826796A270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{A7D75AB7-B047-3448-8A7B-4FE35F9227AE}"/>
   </bookViews>
@@ -1550,7 +1550,7 @@
     <t>K010300981246</t>
   </si>
   <si>
-    <t>T0SMKTH*</t>
+    <t>T0SMKTH#</t>
   </si>
 </sst>
 </file>
@@ -1927,7 +1927,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G247"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>